<commit_message>
try changes for sulphuric acid
</commit_message>
<xml_diff>
--- a/Project10/Project10.xlsx
+++ b/Project10/Project10.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edoardocabiati/Desktop/Cose_brutte_PoliMI/V_anno/II_semestre/Molecular_Modeling_for_Process_Engineering/MMfP/Project10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CEE2C13-F601-8641-BE95-574EB1122FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EFDA6A-C3F3-D546-911A-27826EBD9153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{C3F028D6-4602-7440-949B-282058AFB94C}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C3F028D6-4602-7440-949B-282058AFB94C}"/>
   </bookViews>
   <sheets>
     <sheet name="ions" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="61">
   <si>
     <r>
       <t>1.  HO</t>
@@ -63,16 +64,7 @@
     </r>
   </si>
   <si>
-    <t>G gas</t>
-  </si>
-  <si>
-    <t>G solution</t>
-  </si>
-  <si>
     <t>err %</t>
-  </si>
-  <si>
-    <t>exp. ∆𝐺sol</t>
   </si>
   <si>
     <t>TABLE OF CONSTANTS</t>
@@ -684,6 +676,216 @@
     <t>[KJ/mol]</t>
   </si>
   <si>
+    <t>SCF gas</t>
+  </si>
+  <si>
+    <t>SCF solution</t>
+  </si>
+  <si>
+    <t>CH3COOH</t>
+  </si>
+  <si>
+    <t>CH3COO-</t>
+  </si>
+  <si>
+    <t>H2O4S</t>
+  </si>
+  <si>
+    <t>HO4S-</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>H3O+</t>
+  </si>
+  <si>
+    <t>sulphuric acid</t>
+  </si>
+  <si>
+    <t>acetic acid</t>
+  </si>
+  <si>
+    <t>water and hydronium</t>
+  </si>
+  <si>
+    <r>
+      <t>G°</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>gas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Hartrees]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Acetic acid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> described</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∆𝐺</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>gas</t>
+    </r>
+  </si>
+  <si>
+    <t>Hartrees</t>
+  </si>
+  <si>
+    <r>
+      <t>∆𝐺</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>solv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Hartrees]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∆𝐺</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>solv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [kJ/mol]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∆𝐺</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>solv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [kcal/mol]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>G°</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>sol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Hartrees]</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>∆𝐺</t>
     </r>
@@ -695,8 +897,14 @@
         <color theme="1"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t>sol</t>
-    </r>
+      <t>solv</t>
+    </r>
+  </si>
+  <si>
+    <t>exp. ∆𝐺solv</t>
+  </si>
+  <si>
+    <t>exp. ∆𝐺solv [kcal/mol]</t>
   </si>
 </sst>
 </file>
@@ -707,7 +915,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -740,6 +948,12 @@
       <b/>
       <vertAlign val="subscript"/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
@@ -883,8 +1097,21 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,8 +1166,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1304,84 +1549,237 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="21" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="15" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="22" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="16" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="22" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1415,21 +1813,64 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1985,7 +2426,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>403411</xdr:colOff>
+      <xdr:colOff>237067</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>149412</xdr:rowOff>
     </xdr:from>
@@ -2008,8 +2449,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14761882" y="8352118"/>
-          <a:ext cx="3496236" cy="1016000"/>
+          <a:off x="14681200" y="8345145"/>
+          <a:ext cx="3700432" cy="1013012"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2044,7 +2485,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1800"/>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
             <a:t>BASIS SET</a:t>
           </a:r>
           <a:r>
@@ -2066,8 +2507,12 @@
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
+            <a:t>THEORY LEVEL</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1800" baseline="0"/>
-            <a:t>THEORY LEVEL: </a:t>
+            <a:t>: </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" baseline="0">
@@ -2080,8 +2525,12 @@
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>SCRF method</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1800"/>
-            <a:t>SCRF method: </a:t>
+            <a:t>: </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800">
@@ -2089,7 +2538,693 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>SMD</a:t>
+            <a:t>SMD - water</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>79376</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>141110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>776112</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB03F5FA-D674-0AA8-C076-350A2C1C8939}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14507987" y="6067777"/>
+          <a:ext cx="8184444" cy="732014"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>NOTE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>: The</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> way used to calculate the Gibbs free energies </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>requires the approximation that the thermochemical energy correction (arising from the hessian diagonalization) is equal in both geometries, which can be used for most of the cases.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>103188</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>103187</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E68CF1D6-8ABF-EF8D-17F0-3958B9837480}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8247063" y="6373812"/>
+          <a:ext cx="2095500" cy="674688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>estimated as</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> internal eletronic energy + thermal energy</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3615D3F6-7E10-179D-4F4E-C2703493A404}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6945313" y="7350125"/>
+          <a:ext cx="0" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DF932CD-7BCA-4C40-8D53-899F79CCAA1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7818437" y="7366000"/>
+          <a:ext cx="0" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>904874</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>134937</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5B93A37-0B62-2BDD-F321-1134FF36A340}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6294437" y="7881937"/>
+          <a:ext cx="1047750" cy="277813"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>over</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>estimated</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>168274</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>420688</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9CA4756-D5F0-E44D-BD18-6F648720A16F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7486649" y="7875587"/>
+          <a:ext cx="1077914" cy="292101"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>under</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>estimated</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>222251</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4CCA864-F19A-5EF4-7A91-A13C8948B06C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6532564" y="8278813"/>
+          <a:ext cx="1833562" cy="627062"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>we will</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> be using these experimatal values from this point on</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>337889</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>46605</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>723317</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>36168</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3C7DB2-DDB6-B1CD-B564-425A074EA5AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1165137" y="9705596"/>
+          <a:ext cx="7772400" cy="1178004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>20189</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>197665</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>74774</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123982</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94EE1A79-909B-2F46-BC53-3D80EEFCD50B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6410894" y="4398434"/>
+          <a:ext cx="3669201" cy="1009074"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>BASIS SET</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 6-31+g(d,p)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
+            <a:t>THEORY LEVEL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DFT (B3LYP)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>SCRF method</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>SMD - water</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2418,8 +3553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25149F39-B11C-7A4B-AEA4-4056C843DDDF}">
   <dimension ref="A3:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="D22" zoomScale="106" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2446,11 +3581,11 @@
     </row>
     <row r="5" spans="1:22" ht="23" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4"/>
       <c r="D5" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -2461,13 +3596,13 @@
       <c r="K5" s="6"/>
       <c r="L5" s="7"/>
       <c r="N5" s="8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="10"/>
       <c r="S5" s="11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
@@ -2475,72 +3610,72 @@
     </row>
     <row r="6" spans="1:22" ht="32" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="15">
         <v>6.0221399999999997E+23</v>
       </c>
       <c r="D6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="J6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="K6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="L6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="N6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="O6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="P6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="Q6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="S6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="U6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="22" t="s">
+      <c r="V6" s="25" t="s">
         <v>22</v>
-      </c>
-      <c r="S6" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="U6" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="V6" s="25" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="22" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="27">
         <v>8.3143999999999991</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" s="29">
         <v>1</v>
@@ -2567,7 +3702,7 @@
         <v>6579660000000000</v>
       </c>
       <c r="N7" s="32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O7" s="33">
         <v>1</v>
@@ -2579,7 +3714,7 @@
         <v>5.2917999999999999E-11</v>
       </c>
       <c r="S7" s="35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T7" s="36">
         <v>1</v>
@@ -2594,13 +3729,13 @@
     </row>
     <row r="8" spans="1:22" ht="22" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" s="40">
         <v>1.38065E-23</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E8" s="41">
         <v>3.6750199999999997E-2</v>
@@ -2627,7 +3762,7 @@
         <v>241804000000000</v>
       </c>
       <c r="N8" s="32" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O8" s="45">
         <v>1.8897299999999999</v>
@@ -2639,7 +3774,7 @@
         <v>1E-10</v>
       </c>
       <c r="S8" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T8" s="37">
         <v>1.098E+30</v>
@@ -2654,13 +3789,13 @@
     </row>
     <row r="9" spans="1:22" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="46">
         <v>1.6021760000000001E-16</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9" s="41">
         <v>4.5563300000000003E-6</v>
@@ -2687,7 +3822,7 @@
         <v>29979300000</v>
       </c>
       <c r="N9" s="47" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="O9" s="48">
         <v>18900000000</v>
@@ -2699,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="50" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="T9" s="51">
         <f>U9*T8</f>
@@ -2714,13 +3849,13 @@
     </row>
     <row r="10" spans="1:22" ht="21" x14ac:dyDescent="0.3">
       <c r="A10" s="53" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" s="54">
         <v>9.1092999999999998E-31</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E10" s="41">
         <v>1.59362E-3</v>
@@ -2749,13 +3884,13 @@
     </row>
     <row r="11" spans="1:22" ht="22" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="55">
         <v>8.8541799999999997E-12</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E11" s="41">
         <v>3.8088E-4</v>
@@ -2784,13 +3919,13 @@
     </row>
     <row r="12" spans="1:22" ht="22" x14ac:dyDescent="0.3">
       <c r="A12" s="53" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="54">
         <v>5.2917700000000002E-12</v>
       </c>
       <c r="D12" s="56" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E12" s="41">
         <v>3.1667800000000002E-6</v>
@@ -2819,14 +3954,14 @@
     </row>
     <row r="13" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" s="57">
         <f>298.15</f>
         <v>298.14999999999998</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" s="41">
         <v>2.294E+17</v>
@@ -2855,13 +3990,13 @@
     </row>
     <row r="14" spans="1:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" s="58">
         <v>6.626068E-34</v>
       </c>
       <c r="D14" s="59" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E14" s="60">
         <v>1.5198300000000001E-16</v>
@@ -2888,7 +4023,7 @@
     </row>
     <row r="15" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" s="63">
         <v>1</v>
@@ -2896,7 +4031,7 @@
     </row>
     <row r="16" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="57">
         <v>101325</v>
@@ -2904,7 +4039,7 @@
     </row>
     <row r="17" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="64">
         <v>299792459</v>
@@ -2930,24 +4065,24 @@
     <row r="22" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:13" ht="22" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G23" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="76" t="s">
         <v>1</v>
-      </c>
-      <c r="H23" s="75" t="s">
-        <v>2</v>
-      </c>
-      <c r="I23" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="J23" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="K23" s="76" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F24" s="80" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G24">
         <v>-150.952115397</v>
@@ -2962,7 +4097,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F25" s="81" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G25">
         <f>G24*$H$7</f>
@@ -2979,7 +4114,7 @@
     </row>
     <row r="26" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F26" s="82" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G26">
         <f>G24*$I$7</f>
@@ -2997,7 +4132,7 @@
     <row r="30" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="65" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C31" s="66"/>
       <c r="D31" s="66"/>
@@ -3014,24 +4149,24 @@
     <row r="33" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G34" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J34" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="K34" s="76" t="s">
         <v>1</v>
-      </c>
-      <c r="H34" s="75" t="s">
-        <v>2</v>
-      </c>
-      <c r="I34" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="J34" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="K34" s="76" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F35" s="77" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G35">
         <v>-55.909251517100003</v>
@@ -3046,7 +4181,7 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F36" s="78" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G36">
         <f>G35*$H$7</f>
@@ -3063,7 +4198,7 @@
     </row>
     <row r="37" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F37" s="79" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G37">
         <f>G35*$I$7</f>
@@ -3081,7 +4216,7 @@
     <row r="41" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:13" ht="27" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="68" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C42" s="69"/>
       <c r="D42" s="69"/>
@@ -3098,24 +4233,24 @@
     <row r="44" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:13" ht="22" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G45" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="H45" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="I45" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J45" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="K45" s="76" t="s">
         <v>1</v>
-      </c>
-      <c r="H45" s="75" t="s">
-        <v>2</v>
-      </c>
-      <c r="I45" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="J45" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="K45" s="76" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F46" s="77" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G46">
         <v>-115.115520549</v>
@@ -3130,7 +4265,7 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F47" s="78" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G47">
         <f>G46*$H$7</f>
@@ -3147,7 +4282,7 @@
     </row>
     <row r="48" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F48" s="79" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G48">
         <f>G46*$I$7</f>
@@ -3171,4 +4306,736 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2161192-A836-A949-8E9C-35A7B609FA1C}">
+  <dimension ref="A3:V56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="156" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
+      <c r="N5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="10"/>
+      <c r="S5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="13"/>
+    </row>
+    <row r="6" spans="1:22" ht="32" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15">
+        <v>6.0221399999999997E+23</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="V6" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="22" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="27">
+        <v>8.3143999999999991</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="29">
+        <v>1</v>
+      </c>
+      <c r="F7" s="30">
+        <v>27.210699999999999</v>
+      </c>
+      <c r="G7" s="30">
+        <v>219474.63</v>
+      </c>
+      <c r="H7" s="30">
+        <v>627.50300000000004</v>
+      </c>
+      <c r="I7" s="30">
+        <v>2625.5</v>
+      </c>
+      <c r="J7" s="30">
+        <v>315777</v>
+      </c>
+      <c r="K7" s="30">
+        <v>4.3599999999999999E-18</v>
+      </c>
+      <c r="L7" s="31">
+        <v>6579660000000000</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="33">
+        <v>1</v>
+      </c>
+      <c r="P7" s="33">
+        <v>0.52917999956390005</v>
+      </c>
+      <c r="Q7" s="34">
+        <v>5.2917999999999999E-11</v>
+      </c>
+      <c r="S7" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="36">
+        <v>1</v>
+      </c>
+      <c r="U7" s="37">
+        <v>9.1093800000000005E-31</v>
+      </c>
+      <c r="V7" s="38">
+        <f>U7*V8</f>
+        <v>5.4875783132530122E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="22" x14ac:dyDescent="0.3">
+      <c r="A8" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="40">
+        <v>1.38065E-23</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="41">
+        <v>3.6750199999999997E-2</v>
+      </c>
+      <c r="F8" s="42">
+        <v>1</v>
+      </c>
+      <c r="G8" s="42">
+        <v>8065.73</v>
+      </c>
+      <c r="H8" s="42">
+        <v>23.0609</v>
+      </c>
+      <c r="I8" s="42">
+        <v>96.486900000000006</v>
+      </c>
+      <c r="J8" s="42">
+        <v>11604.9</v>
+      </c>
+      <c r="K8" s="43">
+        <v>1.5999999999999999E-19</v>
+      </c>
+      <c r="L8" s="44">
+        <v>241804000000000</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="45">
+        <v>1.8897299999999999</v>
+      </c>
+      <c r="P8" s="33">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="34">
+        <v>1E-10</v>
+      </c>
+      <c r="S8" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8" s="37">
+        <v>1.098E+30</v>
+      </c>
+      <c r="U8" s="36">
+        <v>1</v>
+      </c>
+      <c r="V8" s="38">
+        <f>1/U9</f>
+        <v>6.0240963855421691E+26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="46">
+        <v>1.6021760000000001E-16</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="41">
+        <v>4.5563300000000003E-6</v>
+      </c>
+      <c r="F9" s="42">
+        <v>1.23981E-4</v>
+      </c>
+      <c r="G9" s="42">
+        <v>1</v>
+      </c>
+      <c r="H9" s="42">
+        <v>2.8590999999999998E-3</v>
+      </c>
+      <c r="I9" s="42">
+        <v>1.1963E-2</v>
+      </c>
+      <c r="J9" s="42">
+        <v>1.42879</v>
+      </c>
+      <c r="K9" s="42">
+        <v>1.9863000000000001E-23</v>
+      </c>
+      <c r="L9" s="44">
+        <v>29979300000</v>
+      </c>
+      <c r="N9" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="48">
+        <v>18900000000</v>
+      </c>
+      <c r="P9" s="48">
+        <v>10000000000</v>
+      </c>
+      <c r="Q9" s="49">
+        <v>1</v>
+      </c>
+      <c r="S9" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="T9" s="51">
+        <f>U9*T8</f>
+        <v>1822.6799999999998</v>
+      </c>
+      <c r="U9" s="51">
+        <v>1.6599999999999999E-27</v>
+      </c>
+      <c r="V9" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="21" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="54">
+        <v>9.1092999999999998E-31</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="41">
+        <v>1.59362E-3</v>
+      </c>
+      <c r="F10" s="42">
+        <v>4.3363400000000003E-2</v>
+      </c>
+      <c r="G10" s="42">
+        <v>349.75700000000001</v>
+      </c>
+      <c r="H10" s="42">
+        <v>1</v>
+      </c>
+      <c r="I10" s="42">
+        <v>4.1840000000000002</v>
+      </c>
+      <c r="J10" s="42">
+        <v>503.22800000000001</v>
+      </c>
+      <c r="K10" s="42">
+        <v>6.9500000000000005E-21</v>
+      </c>
+      <c r="L10" s="44">
+        <v>10485400000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="22" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="55">
+        <v>8.8541799999999997E-12</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="41">
+        <v>3.8088E-4</v>
+      </c>
+      <c r="F11" s="42">
+        <v>1.0364099999999999E-2</v>
+      </c>
+      <c r="G11" s="42">
+        <v>83.593000000000004</v>
+      </c>
+      <c r="H11" s="42">
+        <v>0.23900099999999999</v>
+      </c>
+      <c r="I11" s="42">
+        <v>1</v>
+      </c>
+      <c r="J11" s="42">
+        <v>120.274</v>
+      </c>
+      <c r="K11" s="42">
+        <v>1.6599999999999999E-21</v>
+      </c>
+      <c r="L11" s="44">
+        <v>2506070000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="22" x14ac:dyDescent="0.3">
+      <c r="A12" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="54">
+        <v>5.2917700000000002E-12</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="41">
+        <v>3.1667800000000002E-6</v>
+      </c>
+      <c r="F12" s="42">
+        <v>8.6170500000000004E-5</v>
+      </c>
+      <c r="G12" s="42">
+        <v>0.69502799999999998</v>
+      </c>
+      <c r="H12" s="42">
+        <v>1.9872000000000002E-3</v>
+      </c>
+      <c r="I12" s="42">
+        <v>8.3140000000000002E-3</v>
+      </c>
+      <c r="J12" s="42">
+        <v>1</v>
+      </c>
+      <c r="K12" s="42">
+        <v>1.38054E-23</v>
+      </c>
+      <c r="L12" s="44">
+        <v>20836400000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="57">
+        <f>298.15</f>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="41">
+        <v>2.294E+17</v>
+      </c>
+      <c r="F13" s="42">
+        <v>6.24181E+18</v>
+      </c>
+      <c r="G13" s="42">
+        <v>5.0344500000000003E+22</v>
+      </c>
+      <c r="H13" s="42">
+        <v>1.44E+20</v>
+      </c>
+      <c r="I13" s="42">
+        <v>6.02E+20</v>
+      </c>
+      <c r="J13" s="42">
+        <v>7.2435399999999999E+22</v>
+      </c>
+      <c r="K13" s="42">
+        <v>1</v>
+      </c>
+      <c r="L13" s="44">
+        <v>1.5093E+33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="58">
+        <v>6.626068E-34</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="60">
+        <v>1.5198300000000001E-16</v>
+      </c>
+      <c r="F14" s="61">
+        <v>4.13558E-15</v>
+      </c>
+      <c r="G14" s="61">
+        <v>3.3356499999999997E-11</v>
+      </c>
+      <c r="H14" s="61">
+        <v>9.5370000000000002E-14</v>
+      </c>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61">
+        <v>4.7993E-11</v>
+      </c>
+      <c r="K14" s="61">
+        <v>6.62561E-34</v>
+      </c>
+      <c r="L14" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="57">
+        <v>101325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="64">
+        <v>299792459</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="85"/>
+      <c r="E23" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="87"/>
+      <c r="G23" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="89"/>
+    </row>
+    <row r="24" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="90" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="90" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B25" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="95">
+        <v>-700.18973200000005</v>
+      </c>
+      <c r="D25" s="91">
+        <v>-699.69903599999998</v>
+      </c>
+      <c r="E25" s="91">
+        <v>-229.03990999999999</v>
+      </c>
+      <c r="F25" s="91">
+        <v>-228.49106399999999</v>
+      </c>
+      <c r="G25" s="91">
+        <v>-76.409916999999993</v>
+      </c>
+      <c r="H25" s="91">
+        <v>-76.670537999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B26" s="99" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="96">
+        <v>-700.21422299999995</v>
+      </c>
+      <c r="D26" s="92">
+        <v>-699.80740900000001</v>
+      </c>
+      <c r="E26" s="92">
+        <v>-229.051771</v>
+      </c>
+      <c r="F26" s="92">
+        <v>-228.605279</v>
+      </c>
+      <c r="G26" s="92">
+        <v>-76.424204000000003</v>
+      </c>
+      <c r="H26" s="92">
+        <v>-76.824552999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B27" s="99" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="96">
+        <f>C26-C25</f>
+        <v>-2.4490999999898122E-2</v>
+      </c>
+      <c r="D27" s="92">
+        <f t="shared" ref="D27:H27" si="0">D26-D25</f>
+        <v>-0.1083730000000287</v>
+      </c>
+      <c r="E27" s="92">
+        <f t="shared" si="0"/>
+        <v>-1.1861000000010335E-2</v>
+      </c>
+      <c r="F27" s="92">
+        <f t="shared" si="0"/>
+        <v>-0.11421500000000151</v>
+      </c>
+      <c r="G27" s="92">
+        <f t="shared" si="0"/>
+        <v>-1.4287000000010153E-2</v>
+      </c>
+      <c r="H27" s="92">
+        <f t="shared" si="0"/>
+        <v>-0.15401500000000112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B28" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="96">
+        <f>C27*$I$7</f>
+        <v>-64.301120499732519</v>
+      </c>
+      <c r="D28" s="92">
+        <f t="shared" ref="D28:H28" si="1">D27*$I$7</f>
+        <v>-284.53331150007534</v>
+      </c>
+      <c r="E28" s="92">
+        <f t="shared" si="1"/>
+        <v>-31.141055500027136</v>
+      </c>
+      <c r="F28" s="92">
+        <f t="shared" si="1"/>
+        <v>-299.87148250000394</v>
+      </c>
+      <c r="G28" s="92">
+        <f t="shared" si="1"/>
+        <v>-37.510518500026656</v>
+      </c>
+      <c r="H28" s="92">
+        <f t="shared" si="1"/>
+        <v>-404.36638250000294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B29" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="96">
+        <f>C27*$H$7</f>
+        <v>-15.368175972936072</v>
+      </c>
+      <c r="D29" s="92">
+        <f t="shared" ref="D29:H29" si="2">D27*$H$7</f>
+        <v>-68.004382619018017</v>
+      </c>
+      <c r="E29" s="92">
+        <f t="shared" si="2"/>
+        <v>-7.4428130830064863</v>
+      </c>
+      <c r="F29" s="92">
+        <f t="shared" si="2"/>
+        <v>-71.670255145000951</v>
+      </c>
+      <c r="G29" s="92">
+        <f t="shared" si="2"/>
+        <v>-8.9651353610063715</v>
+      </c>
+      <c r="H29" s="92">
+        <f t="shared" si="2"/>
+        <v>-96.644874545000718</v>
+      </c>
+      <c r="I29" s="83"/>
+    </row>
+    <row r="30" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="97"/>
+      <c r="D30" s="93"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="94">
+        <v>-6.32</v>
+      </c>
+      <c r="H30" s="94">
+        <v>-110.4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:9" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="101" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="102"/>
+      <c r="D40" s="102"/>
+      <c r="E40" s="102"/>
+      <c r="F40" s="102"/>
+      <c r="G40" s="102"/>
+      <c r="H40" s="102"/>
+      <c r="I40" s="103"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51">
+        <f>$H$30*$E$10+F27-($G$30*$E$10+E27)</f>
+        <v>-0.26821796959999117</v>
+      </c>
+      <c r="D51">
+        <f>C51*H7</f>
+        <v>-168.30758057790328</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f>-110.3*E10+6.32*E10-306.833763+307.384162</f>
+        <v>0.38469439240003567</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B40:I40"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>